<commit_message>
hardware and electronics design files
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosam\Dropbox\career\companies\columbia\engineering\SCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosam\Documents\repos\electroporation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Diode</t>
   </si>
@@ -32,15 +32,9 @@
     <t>Relay</t>
   </si>
   <si>
-    <t>Wires</t>
-  </si>
-  <si>
     <t>JST Socket</t>
   </si>
   <si>
-    <t>JST Connector</t>
-  </si>
-  <si>
     <t>Signal Generator</t>
   </si>
   <si>
@@ -90,13 +84,85 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/93657A207/ or https://www.mcmaster.com/93657A505/</t>
+  </si>
+  <si>
+    <t>881-RF300-5</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Teledyne-Relays/RF300-5?qs=cFlnt7DBZX%252BJkIFFO4rSPw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Connector-Pre-Crimped-Compatible-JST-PH2-0mm-Inductrix/dp/B08T89ZK2Q/ref=sr_1_5?crid=2KZ2LYUXJW5KR&amp;keywords=dupont+pre+crimped&amp;qid=1677196883&amp;sprefix=dupont+pre+crimped%25252Caps%25252C69&amp;sr=8-5</t>
+  </si>
+  <si>
+    <t>2-pin, 2mm</t>
+  </si>
+  <si>
+    <t>JST Connector Kit</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/S2B-PH-K-S-LF-SN/926626</t>
+  </si>
+  <si>
+    <t>Right Angle</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>455-1719-ND</t>
+  </si>
+  <si>
+    <t>BNC Connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/mueller-electric-co/BU-5100-A-4-0/5801064</t>
+  </si>
+  <si>
+    <t>314-1393-ND</t>
+  </si>
+  <si>
+    <t>Cheaper equivalent on Amazon</t>
+  </si>
+  <si>
+    <t>D-Sub Male</t>
+  </si>
+  <si>
+    <t>D-Sub Female</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-aerospace-defense-and-marine/206794-4/1144251</t>
+  </si>
+  <si>
+    <t>A34501-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-aerospace-defense-and-marine/206795-3/1144252</t>
+  </si>
+  <si>
+    <t>A34502-ND</t>
+  </si>
+  <si>
+    <t>For compatibility with Axon Instruments Part # &lt;?&gt;</t>
+  </si>
+  <si>
+    <t>https://www.harvardapparatus.com/media/brochures/Warner_Microelectrode_Holders.pdf</t>
+  </si>
+  <si>
+    <t>Pipette Holder</t>
+  </si>
+  <si>
+    <t>QSW-T20P</t>
+  </si>
+  <si>
+    <t>Warner Instruments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +186,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,15 +212,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,33 +502,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E15"/>
+  <dimension ref="A4:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
     <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="132.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -459,80 +537,178 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
         <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E12" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E14" r:id="rId6"/>
+    <hyperlink ref="E15" r:id="rId7"/>
+    <hyperlink ref="E16" r:id="rId8"/>
+    <hyperlink ref="E17" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>